<commit_message>
T1: Refactored finally 57c lab, to little update; T2: Init to lab 29
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/Lab2_Cw57c/Final_Sheet/Ex5,6.xlsx
+++ b/Fizyka_Sprawka/Lab2_Cw57c/Final_Sheet/Ex5,6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clouds\OneDrive\GitHub\TempForSchool\Fizyka_Sprawka\Lab2_Cw57c\Final_OnlyToMerge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clouds\OneDrive\GitHub\TempForSchool\Fizyka_Sprawka\Lab2_Cw57c\Final_Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,9 +38,6 @@
     <t>Wartość</t>
   </si>
   <si>
-    <t>Niepewności z programu na lpf, wyskoczył błąd w trakcie liczenia.</t>
-  </si>
-  <si>
     <t>Wnioski</t>
   </si>
   <si>
@@ -52,15 +49,17 @@
   <si>
     <t>Szukałem w wielu miejscach jak nanieść pola niepewności dla wybranych punktów, nie znalazłem</t>
   </si>
+  <si>
+    <t>Tabela 1.2 Obliczone współczynniki prostej najlepszego dopasowania i ich niepewności</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -79,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -124,15 +123,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -164,7 +154,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -176,50 +168,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -231,61 +180,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -308,14 +246,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>268252</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>187570</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>167701</xdr:rowOff>
+      <xdr:rowOff>149212</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1163652" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -323,7 +261,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1592227" y="1501201"/>
+              <a:off x="2720099" y="1493918"/>
               <a:ext cx="1163652" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -484,7 +422,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -492,7 +430,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1592227" y="1501201"/>
+              <a:off x="2720099" y="1493918"/>
               <a:ext cx="1163652" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -555,8 +493,8 @@
       <xdr:rowOff>172915</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="172611" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -650,7 +588,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -715,8 +653,8 @@
       <xdr:rowOff>178776</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="175882" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -810,7 +748,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -875,8 +813,8 @@
       <xdr:rowOff>16853</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="374911" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -1006,7 +944,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -1083,8 +1021,8 @@
       <xdr:rowOff>8059</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="377475" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -1214,7 +1152,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -1291,8 +1229,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="520462" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -1436,7 +1374,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -1527,8 +1465,8 @@
       <xdr:rowOff>181708</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="517193" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -1672,7 +1610,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -1748,6 +1686,287 @@
               <a:endParaRPr lang="en-US">
                 <a:effectLst/>
               </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>214592</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>189940</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2237344" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2747121" y="1736352"/>
+              <a:ext cx="2237344" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑈</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐻</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐵</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∗</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>−348.90898</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US"/>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>4.90694444</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US"/>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2747121" y="1736352"/>
+              <a:ext cx="2237344" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑈</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐻=𝐵_𝑛∗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"−348.90898</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>"+</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"4.90694444</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0"/>
+                <a:t>"</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -2021,331 +2240,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="H28:I28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="C8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19">
-        <v>3.9068999999999998</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1">
+        <v>4.9069444444444308</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="20">
-        <v>-348.91</v>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1">
+        <v>-348.90897605315354</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="13"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="21">
-        <v>7.6029999999999999E-4</v>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3">
+        <v>0.89211199105837014</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="13"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20">
-        <v>9.3939999999999996E-2</v>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3">
+        <v>2.5232737538208241</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="13"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="22">
-        <v>8.0000000000000002E-3</v>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3">
+        <v>0.9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="22">
-        <v>9.4E-2</v>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6">
+        <v>2.6</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="11"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="23">
-        <v>-0.99911207834369453</v>
+      <c r="B15" s="11">
+        <v>0.99822494509225679</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="11"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="11"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16"/>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A18:I20"/>
     <mergeCell ref="A21:I22"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C12:I12"/>
     <mergeCell ref="A1:I7"/>
+    <mergeCell ref="C8:D17"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="A18:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>